<commit_message>
Added servo functionality to the library. Use setServo to manipulate a remote servo drive.
</commit_message>
<xml_diff>
--- a/Protocol.xlsx
+++ b/Protocol.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="29">
   <si>
     <t>Byte 2</t>
   </si>
@@ -41,62 +41,69 @@
   </si>
   <si>
     <t>Byte 3</t>
+  </si>
+  <si>
+    <t>CHK</t>
+  </si>
+  <si>
+    <t>PIN_MODE 0x04</t>
+  </si>
+  <si>
+    <t>PIN_READ 0x02</t>
+  </si>
+  <si>
+    <t>PIN_DIGITAL 0x01</t>
+  </si>
+  <si>
+    <t>SEND</t>
+  </si>
+  <si>
+    <t>RCV</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Byte 1 </t>
+  </si>
+  <si>
+    <t>uint8_t pin</t>
+  </si>
+  <si>
+    <t>uint8_t value</t>
+  </si>
+  <si>
+    <t>PIN_ANALOG 0x02</t>
+  </si>
+  <si>
+    <t>uint16_t value</t>
+  </si>
+  <si>
+    <t>PIN_WRITE 0x01</t>
+  </si>
+  <si>
+    <t>uint8_t sendback_addr</t>
+  </si>
+  <si>
+    <t>Byte 5</t>
+  </si>
+  <si>
+    <t>Direction</t>
+  </si>
+  <si>
+    <t>TRANSMISSION_ERROR 0xFF</t>
+  </si>
+  <si>
+    <t>RCV ERR</t>
+  </si>
+  <si>
+    <t>servoWrite</t>
   </si>
   <si>
     <t>PIN_INPUT 0x01
 PIN_INPUT_PULLUP 0x02
-PIN_OUTPUT 0x04</t>
-  </si>
-  <si>
-    <t>CHK</t>
-  </si>
-  <si>
-    <t>PIN_MODE 0x04</t>
-  </si>
-  <si>
-    <t>PIN_READ 0x02</t>
-  </si>
-  <si>
-    <t>PIN_DIGITAL 0x01</t>
-  </si>
-  <si>
-    <t>SEND</t>
-  </si>
-  <si>
-    <t>RCV</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Byte 1 </t>
-  </si>
-  <si>
-    <t>uint8_t pin</t>
-  </si>
-  <si>
-    <t>uint8_t value</t>
-  </si>
-  <si>
-    <t>PIN_ANALOG 0x02</t>
-  </si>
-  <si>
-    <t>uint16_t value</t>
-  </si>
-  <si>
-    <t>PIN_WRITE 0x01</t>
-  </si>
-  <si>
-    <t>uint8_t sendback_addr</t>
-  </si>
-  <si>
-    <t>Byte 5</t>
-  </si>
-  <si>
-    <t>Direction</t>
-  </si>
-  <si>
-    <t>TRANSMISSION_ERROR 0xFF</t>
-  </si>
-  <si>
-    <t>RCV ERR</t>
+PIN_OUTPUT 0x04
+PIN_SERVO 0x08</t>
+  </si>
+  <si>
+    <t>PIN_SERVO 0x08</t>
   </si>
 </sst>
 </file>
@@ -465,10 +472,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G18"/>
+  <dimension ref="A1:G21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="M19" sqref="M19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -480,13 +487,13 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>7</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>0</v>
@@ -498,7 +505,7 @@
         <v>1</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -506,21 +513,21 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>9</v>
+        <v>27</v>
       </c>
       <c r="D4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -533,56 +540,56 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" t="s">
         <v>12</v>
       </c>
-      <c r="C7" t="s">
-        <v>13</v>
-      </c>
       <c r="D7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" t="s">
         <v>12</v>
       </c>
-      <c r="C8" t="s">
-        <v>13</v>
-      </c>
       <c r="D8" t="s">
+        <v>16</v>
+      </c>
+      <c r="E8" t="s">
         <v>17</v>
       </c>
-      <c r="E8" t="s">
-        <v>18</v>
-      </c>
       <c r="F8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B9" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -592,57 +599,57 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C11" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E11" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F11" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B12" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C12" t="s">
+        <v>18</v>
+      </c>
+      <c r="D12" t="s">
+        <v>16</v>
+      </c>
+      <c r="E12" s="5" t="s">
         <v>19</v>
-      </c>
-      <c r="D12" t="s">
-        <v>17</v>
-      </c>
-      <c r="E12" s="5" t="s">
-        <v>20</v>
       </c>
       <c r="F12" s="5"/>
       <c r="G12" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B13" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C13" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D13" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E13" s="4"/>
       <c r="F13" s="4"/>
@@ -654,22 +661,22 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C15" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D15" t="s">
+        <v>16</v>
+      </c>
+      <c r="E15" t="s">
         <v>17</v>
       </c>
-      <c r="E15" t="s">
-        <v>18</v>
-      </c>
       <c r="F15" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
@@ -679,23 +686,48 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B18" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C18" t="s">
+        <v>18</v>
+      </c>
+      <c r="D18" t="s">
+        <v>16</v>
+      </c>
+      <c r="E18" s="5" t="s">
         <v>19</v>
-      </c>
-      <c r="D18" t="s">
-        <v>17</v>
-      </c>
-      <c r="E18" s="5" t="s">
-        <v>20</v>
       </c>
       <c r="F18" s="5"/>
       <c r="G18" t="s">
-        <v>10</v>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>13</v>
+      </c>
+      <c r="B21" t="s">
+        <v>20</v>
+      </c>
+      <c r="C21" t="s">
+        <v>28</v>
+      </c>
+      <c r="D21" t="s">
+        <v>16</v>
+      </c>
+      <c r="E21" t="s">
+        <v>17</v>
+      </c>
+      <c r="F21" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>